<commit_message>
add UML and update porgress table
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C566C5C-9F9D-4965-857D-3D51F69CBCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF538EAA-4BBC-493B-A3A0-2B04CA6BAB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>在此工作表中创建项目日程安排。
 在单元格 B1 中输入此项目的标题。
@@ -195,10 +195,6 @@
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>原型图</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
     <t>阶段 1 项目原型设计</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
@@ -231,14 +227,6 @@
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>前端css和js</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
-    <t>前后端调试接口</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
     <t>阶段 3 前端css和js添加+前后端调试接口+爬虫</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
@@ -260,6 +248,54 @@
   </si>
   <si>
     <t>前端收藏夹功能优化</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端接口接入</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端样式css</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端页面逻辑js</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>李桢</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>张伟泽</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>前后端接协调口</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>原型图设计和优化</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>小程序分享页面优化</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>阶段 5 小程序测试</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发人员内测</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽取用户外测</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>试用用户</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
 </sst>
@@ -519,7 +555,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,6 +807,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -1044,7 +1092,7 @@
     <xf numFmtId="0" fontId="4" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1312,6 +1360,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="180" fontId="4" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="45" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="45" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="28" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="46" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="46" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="46" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="46" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1921,11 +1996,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL24"/>
+  <dimension ref="A1:BL30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AV10" sqref="AV10"/>
+      <selection pane="bottomLeft" activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2627,7 +2702,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="46"/>
@@ -2635,7 +2710,7 @@
       <c r="F8" s="80"/>
       <c r="G8" s="47"/>
       <c r="H8" s="47" t="str">
-        <f t="shared" ref="H8:H21" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H27" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="6"/>
@@ -2700,10 +2775,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="48">
         <v>1</v>
@@ -2783,7 +2858,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="50"/>
@@ -2854,10 +2929,10 @@
     <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="16"/>
       <c r="B11" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="51">
         <v>1</v>
@@ -2934,10 +3009,10 @@
     <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="15"/>
       <c r="B12" s="31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="51">
         <v>1</v>
@@ -3015,26 +3090,26 @@
     <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="51">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E13" s="84">
         <f>E11</f>
         <v>44812</v>
       </c>
       <c r="F13" s="84">
-        <f>E13+26</f>
-        <v>44838</v>
+        <f>E13+24</f>
+        <v>44836</v>
       </c>
       <c r="G13" s="47"/>
       <c r="H13" s="47">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -3098,7 +3173,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="53"/>
@@ -3169,26 +3244,26 @@
     <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15"/>
       <c r="B15" s="32" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D15" s="54">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E15" s="87">
         <f>E9+18</f>
         <v>44823</v>
       </c>
       <c r="F15" s="87">
-        <f>E15+15</f>
-        <v>44838</v>
+        <f>E15+10</f>
+        <v>44833</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="47">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -3250,27 +3325,22 @@
     <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15"/>
       <c r="B16" s="32" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D16" s="54">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="E16" s="87">
-        <f>E15</f>
-        <v>44823</v>
+        <v>44825</v>
       </c>
       <c r="F16" s="87">
-        <f>E16+15</f>
         <v>44838</v>
       </c>
       <c r="G16" s="47"/>
-      <c r="H16" s="47">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
+      <c r="H16" s="47"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -3331,27 +3401,22 @@
     <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="15"/>
       <c r="B17" s="32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D17" s="54">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E17" s="87">
-        <f>E15</f>
-        <v>44823</v>
+        <v>44829</v>
       </c>
       <c r="F17" s="87">
-        <f>E17+15</f>
         <v>44838</v>
       </c>
       <c r="G17" s="47"/>
-      <c r="H17" s="47">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
+      <c r="H17" s="47"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -3410,20 +3475,28 @@
       <c r="BL17" s="6"/>
     </row>
     <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="89"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="54">
+        <v>0.9</v>
+      </c>
+      <c r="E18" s="87">
+        <f>E15</f>
+        <v>44823</v>
+      </c>
+      <c r="F18" s="87">
+        <f>E18+20</f>
+        <v>44843</v>
+      </c>
       <c r="G18" s="47"/>
-      <c r="H18" s="47" t="str">
+      <c r="H18" s="47">
         <f t="shared" si="4"/>
-        <v/>
+        <v>21</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -3484,26 +3557,27 @@
     </row>
     <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="15"/>
-      <c r="B19" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="57">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="90">
-        <v>44835</v>
-      </c>
-      <c r="F19" s="90">
-        <f>E19+3</f>
-        <v>44838</v>
+      <c r="B19" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="54">
+        <v>1</v>
+      </c>
+      <c r="E19" s="87">
+        <f>E15</f>
+        <v>44823</v>
+      </c>
+      <c r="F19" s="87">
+        <f>E19+20</f>
+        <v>44843</v>
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="47">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -3564,13 +3638,15 @@
     </row>
     <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="89"/>
       <c r="G20" s="47"/>
       <c r="H20" s="47" t="str">
         <f t="shared" si="4"/>
@@ -3634,87 +3710,546 @@
       <c r="BL20" s="6"/>
     </row>
     <row r="21" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65" t="str">
+      <c r="A21" s="15"/>
+      <c r="B21" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="57">
+        <v>1</v>
+      </c>
+      <c r="E21" s="90">
+        <v>44835</v>
+      </c>
+      <c r="F21" s="90">
+        <f>E21+8</f>
+        <v>44843</v>
+      </c>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="6"/>
+      <c r="AJ21" s="6"/>
+      <c r="AK21" s="6"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="6"/>
+      <c r="AP21" s="6"/>
+      <c r="AQ21" s="6"/>
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="6"/>
+      <c r="AU21" s="6"/>
+      <c r="AV21" s="6"/>
+      <c r="AW21" s="6"/>
+      <c r="AX21" s="6"/>
+      <c r="AY21" s="6"/>
+      <c r="AZ21" s="6"/>
+      <c r="BA21" s="6"/>
+      <c r="BB21" s="6"/>
+      <c r="BC21" s="6"/>
+      <c r="BD21" s="6"/>
+      <c r="BE21" s="6"/>
+      <c r="BF21" s="6"/>
+      <c r="BG21" s="6"/>
+      <c r="BH21" s="6"/>
+      <c r="BI21" s="6"/>
+      <c r="BJ21" s="6"/>
+      <c r="BK21" s="6"/>
+      <c r="BL21" s="6"/>
+    </row>
+    <row r="22" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="15"/>
+      <c r="B22" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="57">
+        <v>1</v>
+      </c>
+      <c r="E22" s="90">
+        <v>44835</v>
+      </c>
+      <c r="F22" s="90">
+        <f>E22+8</f>
+        <v>44843</v>
+      </c>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="6"/>
+      <c r="AJ22" s="6"/>
+      <c r="AK22" s="6"/>
+      <c r="AL22" s="6"/>
+      <c r="AM22" s="6"/>
+      <c r="AN22" s="6"/>
+      <c r="AO22" s="6"/>
+      <c r="AP22" s="6"/>
+      <c r="AQ22" s="6"/>
+      <c r="AR22" s="6"/>
+      <c r="AS22" s="6"/>
+      <c r="AT22" s="6"/>
+      <c r="AU22" s="6"/>
+      <c r="AV22" s="6"/>
+      <c r="AW22" s="6"/>
+      <c r="AX22" s="6"/>
+      <c r="AY22" s="6"/>
+      <c r="AZ22" s="6"/>
+      <c r="BA22" s="6"/>
+      <c r="BB22" s="6"/>
+      <c r="BC22" s="6"/>
+      <c r="BD22" s="6"/>
+      <c r="BE22" s="6"/>
+      <c r="BF22" s="6"/>
+      <c r="BG22" s="6"/>
+      <c r="BH22" s="6"/>
+      <c r="BI22" s="6"/>
+      <c r="BJ22" s="6"/>
+      <c r="BK22" s="6"/>
+      <c r="BL22" s="6"/>
+    </row>
+    <row r="23" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="98"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="8"/>
-      <c r="AE21" s="8"/>
-      <c r="AF21" s="8"/>
-      <c r="AG21" s="8"/>
-      <c r="AH21" s="8"/>
-      <c r="AI21" s="8"/>
-      <c r="AJ21" s="8"/>
-      <c r="AK21" s="8"/>
-      <c r="AL21" s="8"/>
-      <c r="AM21" s="8"/>
-      <c r="AN21" s="8"/>
-      <c r="AO21" s="8"/>
-      <c r="AP21" s="8"/>
-      <c r="AQ21" s="8"/>
-      <c r="AR21" s="8"/>
-      <c r="AS21" s="8"/>
-      <c r="AT21" s="8"/>
-      <c r="AU21" s="8"/>
-      <c r="AV21" s="8"/>
-      <c r="AW21" s="8"/>
-      <c r="AX21" s="8"/>
-      <c r="AY21" s="8"/>
-      <c r="AZ21" s="8"/>
-      <c r="BA21" s="8"/>
-      <c r="BB21" s="8"/>
-      <c r="BC21" s="8"/>
-      <c r="BD21" s="8"/>
-      <c r="BE21" s="8"/>
-      <c r="BF21" s="8"/>
-      <c r="BG21" s="8"/>
-      <c r="BH21" s="8"/>
-      <c r="BI21" s="8"/>
-      <c r="BJ21" s="8"/>
-      <c r="BK21" s="8"/>
-      <c r="BL21" s="8"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="6"/>
+      <c r="AK23" s="6"/>
+      <c r="AL23" s="6"/>
+      <c r="AM23" s="6"/>
+      <c r="AN23" s="6"/>
+      <c r="AO23" s="6"/>
+      <c r="AP23" s="6"/>
+      <c r="AQ23" s="6"/>
+      <c r="AR23" s="6"/>
+      <c r="AS23" s="6"/>
+      <c r="AT23" s="6"/>
+      <c r="AU23" s="6"/>
+      <c r="AV23" s="6"/>
+      <c r="AW23" s="6"/>
+      <c r="AX23" s="6"/>
+      <c r="AY23" s="6"/>
+      <c r="AZ23" s="6"/>
+      <c r="BA23" s="6"/>
+      <c r="BB23" s="6"/>
+      <c r="BC23" s="6"/>
+      <c r="BD23" s="6"/>
+      <c r="BE23" s="6"/>
+      <c r="BF23" s="6"/>
+      <c r="BG23" s="6"/>
+      <c r="BH23" s="6"/>
+      <c r="BI23" s="6"/>
+      <c r="BJ23" s="6"/>
+      <c r="BK23" s="6"/>
+      <c r="BL23" s="6"/>
     </row>
-    <row r="22" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G22" s="4"/>
+    <row r="24" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="102" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="103" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="104">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="105">
+        <v>44844</v>
+      </c>
+      <c r="F24" s="105">
+        <f>E24+4</f>
+        <v>44848</v>
+      </c>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="6"/>
+      <c r="AK24" s="6"/>
+      <c r="AL24" s="6"/>
+      <c r="AM24" s="6"/>
+      <c r="AN24" s="6"/>
+      <c r="AO24" s="6"/>
+      <c r="AP24" s="6"/>
+      <c r="AQ24" s="6"/>
+      <c r="AR24" s="6"/>
+      <c r="AS24" s="6"/>
+      <c r="AT24" s="6"/>
+      <c r="AU24" s="6"/>
+      <c r="AV24" s="6"/>
+      <c r="AW24" s="6"/>
+      <c r="AX24" s="6"/>
+      <c r="AY24" s="6"/>
+      <c r="AZ24" s="6"/>
+      <c r="BA24" s="6"/>
+      <c r="BB24" s="6"/>
+      <c r="BC24" s="6"/>
+      <c r="BD24" s="6"/>
+      <c r="BE24" s="6"/>
+      <c r="BF24" s="6"/>
+      <c r="BG24" s="6"/>
+      <c r="BH24" s="6"/>
+      <c r="BI24" s="6"/>
+      <c r="BJ24" s="6"/>
+      <c r="BK24" s="6"/>
+      <c r="BL24" s="6"/>
     </row>
-    <row r="23" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="66"/>
-      <c r="F23" s="67"/>
+    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="16"/>
+      <c r="B25" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="104">
+        <v>0</v>
+      </c>
+      <c r="E25" s="105">
+        <v>44849</v>
+      </c>
+      <c r="F25" s="105">
+        <v>44857</v>
+      </c>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="6"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="6"/>
+      <c r="AP25" s="6"/>
+      <c r="AQ25" s="6"/>
+      <c r="AR25" s="6"/>
+      <c r="AS25" s="6"/>
+      <c r="AT25" s="6"/>
+      <c r="AU25" s="6"/>
+      <c r="AV25" s="6"/>
+      <c r="AW25" s="6"/>
+      <c r="AX25" s="6"/>
+      <c r="AY25" s="6"/>
+      <c r="AZ25" s="6"/>
+      <c r="BA25" s="6"/>
+      <c r="BB25" s="6"/>
+      <c r="BC25" s="6"/>
+      <c r="BD25" s="6"/>
+      <c r="BE25" s="6"/>
+      <c r="BF25" s="6"/>
+      <c r="BG25" s="6"/>
+      <c r="BH25" s="6"/>
+      <c r="BI25" s="6"/>
+      <c r="BJ25" s="6"/>
+      <c r="BK25" s="6"/>
+      <c r="BL25" s="6"/>
     </row>
-    <row r="24" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="68"/>
+    <row r="26" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="6"/>
+      <c r="AH26" s="6"/>
+      <c r="AI26" s="6"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="6"/>
+      <c r="AL26" s="6"/>
+      <c r="AM26" s="6"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="6"/>
+      <c r="AP26" s="6"/>
+      <c r="AQ26" s="6"/>
+      <c r="AR26" s="6"/>
+      <c r="AS26" s="6"/>
+      <c r="AT26" s="6"/>
+      <c r="AU26" s="6"/>
+      <c r="AV26" s="6"/>
+      <c r="AW26" s="6"/>
+      <c r="AX26" s="6"/>
+      <c r="AY26" s="6"/>
+      <c r="AZ26" s="6"/>
+      <c r="BA26" s="6"/>
+      <c r="BB26" s="6"/>
+      <c r="BC26" s="6"/>
+      <c r="BD26" s="6"/>
+      <c r="BE26" s="6"/>
+      <c r="BF26" s="6"/>
+      <c r="BG26" s="6"/>
+      <c r="BH26" s="6"/>
+      <c r="BI26" s="6"/>
+      <c r="BJ26" s="6"/>
+      <c r="BK26" s="6"/>
+      <c r="BL26" s="6"/>
+    </row>
+    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="61"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8"/>
+      <c r="AB27" s="8"/>
+      <c r="AC27" s="8"/>
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="8"/>
+      <c r="AF27" s="8"/>
+      <c r="AG27" s="8"/>
+      <c r="AH27" s="8"/>
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="8"/>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="8"/>
+      <c r="AM27" s="8"/>
+      <c r="AN27" s="8"/>
+      <c r="AO27" s="8"/>
+      <c r="AP27" s="8"/>
+      <c r="AQ27" s="8"/>
+      <c r="AR27" s="8"/>
+      <c r="AS27" s="8"/>
+      <c r="AT27" s="8"/>
+      <c r="AU27" s="8"/>
+      <c r="AV27" s="8"/>
+      <c r="AW27" s="8"/>
+      <c r="AX27" s="8"/>
+      <c r="AY27" s="8"/>
+      <c r="AZ27" s="8"/>
+      <c r="BA27" s="8"/>
+      <c r="BB27" s="8"/>
+      <c r="BC27" s="8"/>
+      <c r="BD27" s="8"/>
+      <c r="BE27" s="8"/>
+      <c r="BF27" s="8"/>
+      <c r="BG27" s="8"/>
+      <c r="BH27" s="8"/>
+      <c r="BI27" s="8"/>
+      <c r="BJ27" s="8"/>
+      <c r="BK27" s="8"/>
+      <c r="BL27" s="8"/>
+    </row>
+    <row r="28" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="66"/>
+      <c r="F29" s="67"/>
+    </row>
+    <row r="30" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3731,7 +4266,7 @@
     <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <phoneticPr fontId="37" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D21">
+  <conditionalFormatting sqref="D7:D27">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3745,12 +4280,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL21">
+  <conditionalFormatting sqref="I5:BL27">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL21">
+  <conditionalFormatting sqref="I7:BL27">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -3785,7 +4320,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D21</xm:sqref>
+          <xm:sqref>D7:D27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>